<commit_message>
update: atualiza script SQL
</commit_message>
<xml_diff>
--- a/ajustes/Novas demandas.xlsx
+++ b/ajustes/Novas demandas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos Ciência de Dados\cr_novacap\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos Ciência de Dados\cr_novacap\ajustes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4728F8-CEA1-43B2-9847-9CDA17830C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4956E059-7666-4AF9-AB77-801A4E2E373A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{0B16755F-254A-4C4A-AAAD-7AB7C4BF30FE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="198">
   <si>
     <t>ID ORIGINAL</t>
   </si>
@@ -641,7 +641,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="00000&quot;-&quot;########&quot;/&quot;####&quot;-&quot;##"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -918,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -960,6 +960,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -978,40 +998,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="00000&quot;-&quot;########&quot;/&quot;####&quot;-&quot;##"/>
@@ -1408,10 +1407,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1421,8 +1420,8 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="5" t="s">
         <v>31</v>
       </c>
@@ -1430,10 +1429,10 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="32">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1443,8 +1442,8 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1452,8 +1451,8 @@
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
@@ -1461,8 +1460,8 @@
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1470,8 +1469,8 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1479,8 +1478,8 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="4" t="s">
         <v>37</v>
       </c>
@@ -1488,10 +1487,10 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="32">
         <v>3</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1501,8 +1500,8 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1510,8 +1509,8 @@
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
@@ -1519,8 +1518,8 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
@@ -1528,8 +1527,8 @@
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1537,8 +1536,8 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="4" t="s">
         <v>43</v>
       </c>
@@ -1546,10 +1545,10 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+      <c r="A16" s="32">
         <v>4</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1559,8 +1558,8 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1568,8 +1567,8 @@
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="2" t="s">
         <v>46</v>
       </c>
@@ -1577,8 +1576,8 @@
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="4" t="s">
         <v>47</v>
       </c>
@@ -1612,10 +1611,10 @@
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="22">
+      <c r="A22" s="32">
         <v>7</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1625,8 +1624,8 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="1" t="s">
         <v>51</v>
       </c>
@@ -1634,8 +1633,8 @@
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1643,8 +1642,8 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
@@ -1652,8 +1651,8 @@
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
@@ -1661,8 +1660,8 @@
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="2" t="s">
         <v>55</v>
       </c>
@@ -1670,8 +1669,8 @@
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
-      <c r="B28" s="21"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="4" t="s">
         <v>56</v>
       </c>
@@ -1679,10 +1678,10 @@
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="A29" s="32">
         <v>8</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -1692,8 +1691,8 @@
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1701,8 +1700,8 @@
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="20"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="2" t="s">
         <v>59</v>
       </c>
@@ -1710,8 +1709,8 @@
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="20"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
@@ -1719,8 +1718,8 @@
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="20"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="2" t="s">
         <v>61</v>
       </c>
@@ -1728,8 +1727,8 @@
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
-      <c r="B34" s="21"/>
+      <c r="A34" s="34"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="4" t="s">
         <v>62</v>
       </c>
@@ -1737,10 +1736,10 @@
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
+      <c r="A35" s="32">
         <v>9</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -1750,8 +1749,8 @@
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="20"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="2" t="s">
         <v>64</v>
       </c>
@@ -1759,8 +1758,8 @@
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="20"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="2" t="s">
         <v>65</v>
       </c>
@@ -1768,8 +1767,8 @@
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="21"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="31"/>
       <c r="C38" s="4" t="s">
         <v>66</v>
       </c>
@@ -1790,10 +1789,10 @@
       <c r="E39" s="13"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="22">
+      <c r="A40" s="32">
         <v>11</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -1803,8 +1802,8 @@
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="20"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="2" t="s">
         <v>69</v>
       </c>
@@ -1812,8 +1811,8 @@
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="20"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="2" t="s">
         <v>70</v>
       </c>
@@ -1821,8 +1820,8 @@
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
-      <c r="B43" s="21"/>
+      <c r="A43" s="34"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="4" t="s">
         <v>71</v>
       </c>
@@ -1830,10 +1829,10 @@
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="22">
+      <c r="A44" s="32">
         <v>12</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -1843,8 +1842,8 @@
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="33"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="2" t="s">
         <v>73</v>
       </c>
@@ -1852,8 +1851,8 @@
       <c r="E45" s="15"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
-      <c r="B46" s="21"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="4" t="s">
         <v>74</v>
       </c>
@@ -1861,10 +1860,10 @@
       <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="A47" s="32">
         <v>13</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -1874,8 +1873,8 @@
       <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="20"/>
+      <c r="A48" s="33"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="2" t="s">
         <v>76</v>
       </c>
@@ -1883,8 +1882,8 @@
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="20"/>
+      <c r="A49" s="33"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="2" t="s">
         <v>77</v>
       </c>
@@ -1892,8 +1891,8 @@
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="20"/>
+      <c r="A50" s="33"/>
+      <c r="B50" s="30"/>
       <c r="C50" s="2" t="s">
         <v>78</v>
       </c>
@@ -1901,8 +1900,8 @@
       <c r="E50" s="3"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="20"/>
+      <c r="A51" s="33"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="2" t="s">
         <v>79</v>
       </c>
@@ -1910,8 +1909,8 @@
       <c r="E51" s="3"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24"/>
-      <c r="B52" s="21"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="4" t="s">
         <v>80</v>
       </c>
@@ -1919,10 +1918,10 @@
       <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
+      <c r="A53" s="32">
         <v>14</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -1932,8 +1931,8 @@
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="20"/>
+      <c r="A54" s="33"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="1" t="s">
         <v>82</v>
       </c>
@@ -1941,8 +1940,8 @@
       <c r="E54" s="3"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="20"/>
+      <c r="A55" s="33"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="1" t="s">
         <v>83</v>
       </c>
@@ -1950,8 +1949,8 @@
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
-      <c r="B56" s="21"/>
+      <c r="A56" s="34"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="4" t="s">
         <v>84</v>
       </c>
@@ -1959,10 +1958,10 @@
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
+      <c r="A57" s="32">
         <v>15</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -1972,8 +1971,8 @@
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="20"/>
+      <c r="A58" s="33"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="2" t="s">
         <v>86</v>
       </c>
@@ -1981,8 +1980,8 @@
       <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
-      <c r="B59" s="21"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="4" t="s">
         <v>87</v>
       </c>
@@ -1990,10 +1989,10 @@
       <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
+      <c r="A60" s="32">
         <v>16</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="9" t="s">
@@ -2003,8 +2002,8 @@
       <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24"/>
-      <c r="B61" s="21"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="4" t="s">
         <v>89</v>
       </c>
@@ -2012,10 +2011,10 @@
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
+      <c r="A62" s="32">
         <v>17</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -2025,8 +2024,8 @@
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
-      <c r="B63" s="20"/>
+      <c r="A63" s="33"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="2" t="s">
         <v>91</v>
       </c>
@@ -2034,8 +2033,8 @@
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="20"/>
+      <c r="A64" s="33"/>
+      <c r="B64" s="30"/>
       <c r="C64" s="2" t="s">
         <v>92</v>
       </c>
@@ -2043,8 +2042,8 @@
       <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-      <c r="B65" s="20"/>
+      <c r="A65" s="33"/>
+      <c r="B65" s="30"/>
       <c r="C65" s="2" t="s">
         <v>93</v>
       </c>
@@ -2052,8 +2051,8 @@
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-      <c r="B66" s="20"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="2" t="s">
         <v>94</v>
       </c>
@@ -2061,8 +2060,8 @@
       <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="24"/>
-      <c r="B67" s="21"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="4" t="s">
         <v>95</v>
       </c>
@@ -2070,10 +2069,10 @@
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="22">
+      <c r="A68" s="32">
         <v>18</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="29" t="s">
         <v>18</v>
       </c>
       <c r="C68" s="9" t="s">
@@ -2083,8 +2082,8 @@
       <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
-      <c r="B69" s="20"/>
+      <c r="A69" s="33"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="2" t="s">
         <v>97</v>
       </c>
@@ -2092,8 +2091,8 @@
       <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
-      <c r="B70" s="20"/>
+      <c r="A70" s="33"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="2" t="s">
         <v>98</v>
       </c>
@@ -2101,8 +2100,8 @@
       <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="24"/>
-      <c r="B71" s="21"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="4" t="s">
         <v>99</v>
       </c>
@@ -2110,10 +2109,10 @@
       <c r="E71" s="6"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
+      <c r="A72" s="32">
         <v>19</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="29" t="s">
         <v>21</v>
       </c>
       <c r="C72" s="9" t="s">
@@ -2123,8 +2122,8 @@
       <c r="E72" s="8"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
-      <c r="B73" s="20"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="2" t="s">
         <v>101</v>
       </c>
@@ -2132,8 +2131,8 @@
       <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="20"/>
+      <c r="A74" s="33"/>
+      <c r="B74" s="30"/>
       <c r="C74" s="2" t="s">
         <v>102</v>
       </c>
@@ -2141,8 +2140,8 @@
       <c r="E74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="20"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="30"/>
       <c r="C75" s="2" t="s">
         <v>103</v>
       </c>
@@ -2150,8 +2149,8 @@
       <c r="E75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="20"/>
+      <c r="A76" s="33"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="2" t="s">
         <v>104</v>
       </c>
@@ -2159,8 +2158,8 @@
       <c r="E76" s="3"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="24"/>
-      <c r="B77" s="21"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="4" t="s">
         <v>105</v>
       </c>
@@ -2168,10 +2167,10 @@
       <c r="E77" s="6"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
+      <c r="A78" s="32">
         <v>20</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="B78" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C78" s="9" t="s">
@@ -2181,8 +2180,8 @@
       <c r="E78" s="8"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="23"/>
-      <c r="B79" s="20"/>
+      <c r="A79" s="33"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="2" t="s">
         <v>107</v>
       </c>
@@ -2190,8 +2189,8 @@
       <c r="E79" s="3"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
-      <c r="B80" s="20"/>
+      <c r="A80" s="33"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="2" t="s">
         <v>108</v>
       </c>
@@ -2199,8 +2198,8 @@
       <c r="E80" s="3"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="20"/>
+      <c r="A81" s="33"/>
+      <c r="B81" s="30"/>
       <c r="C81" s="2" t="s">
         <v>109</v>
       </c>
@@ -2208,8 +2207,8 @@
       <c r="E81" s="3"/>
     </row>
     <row r="82" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="24"/>
-      <c r="B82" s="21"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="4" t="s">
         <v>110</v>
       </c>
@@ -2217,10 +2216,10 @@
       <c r="E82" s="6"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="22">
+      <c r="A83" s="32">
         <v>21</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C83" s="9" t="s">
@@ -2230,8 +2229,8 @@
       <c r="E83" s="8"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="23"/>
-      <c r="B84" s="20"/>
+      <c r="A84" s="33"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="2" t="s">
         <v>112</v>
       </c>
@@ -2239,8 +2238,8 @@
       <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
-      <c r="B85" s="20"/>
+      <c r="A85" s="33"/>
+      <c r="B85" s="30"/>
       <c r="C85" s="2" t="s">
         <v>113</v>
       </c>
@@ -2248,8 +2247,8 @@
       <c r="E85" s="3"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
-      <c r="B86" s="20"/>
+      <c r="A86" s="33"/>
+      <c r="B86" s="30"/>
       <c r="C86" s="2" t="s">
         <v>114</v>
       </c>
@@ -2257,8 +2256,8 @@
       <c r="E86" s="3"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="24"/>
-      <c r="B87" s="21"/>
+      <c r="A87" s="34"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="4" t="s">
         <v>115</v>
       </c>
@@ -2266,10 +2265,10 @@
       <c r="E87" s="6"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="22">
+      <c r="A88" s="32">
         <v>22</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C88" s="9" t="s">
@@ -2279,8 +2278,8 @@
       <c r="E88" s="8"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="23"/>
-      <c r="B89" s="20"/>
+      <c r="A89" s="33"/>
+      <c r="B89" s="30"/>
       <c r="C89" s="2" t="s">
         <v>117</v>
       </c>
@@ -2288,8 +2287,8 @@
       <c r="E89" s="3"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="24"/>
-      <c r="B90" s="21"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="4" t="s">
         <v>118</v>
       </c>
@@ -2310,10 +2309,10 @@
       <c r="E91" s="13"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="22">
+      <c r="A92" s="32">
         <v>24</v>
       </c>
-      <c r="B92" s="19" t="s">
+      <c r="B92" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C92" s="7" t="s">
@@ -2323,8 +2322,8 @@
       <c r="E92" s="8"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
-      <c r="B93" s="20"/>
+      <c r="A93" s="33"/>
+      <c r="B93" s="30"/>
       <c r="C93" s="2" t="s">
         <v>121</v>
       </c>
@@ -2332,8 +2331,8 @@
       <c r="E93" s="3"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
-      <c r="B94" s="20"/>
+      <c r="A94" s="33"/>
+      <c r="B94" s="30"/>
       <c r="C94" s="2" t="s">
         <v>122</v>
       </c>
@@ -2341,8 +2340,8 @@
       <c r="E94" s="3"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
-      <c r="B95" s="20"/>
+      <c r="A95" s="33"/>
+      <c r="B95" s="30"/>
       <c r="C95" s="2" t="s">
         <v>123</v>
       </c>
@@ -2350,8 +2349,8 @@
       <c r="E95" s="3"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
-      <c r="B96" s="20"/>
+      <c r="A96" s="33"/>
+      <c r="B96" s="30"/>
       <c r="C96" s="2" t="s">
         <v>124</v>
       </c>
@@ -2359,8 +2358,8 @@
       <c r="E96" s="3"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="24"/>
-      <c r="B97" s="21"/>
+      <c r="A97" s="34"/>
+      <c r="B97" s="31"/>
       <c r="C97" s="4" t="s">
         <v>125</v>
       </c>
@@ -2385,6 +2384,36 @@
     <sortCondition ref="C2:C98"/>
   </sortState>
   <mergeCells count="40">
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="A62:A67"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="A68:A71"/>
     <mergeCell ref="B88:B90"/>
     <mergeCell ref="A88:A90"/>
     <mergeCell ref="B92:B97"/>
@@ -2395,36 +2424,6 @@
     <mergeCell ref="A78:A82"/>
     <mergeCell ref="B83:B87"/>
     <mergeCell ref="A83:A87"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A22:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="A47:A52"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D96" xr:uid="{612526A2-62F5-4629-8B41-0E38B073389A}">
@@ -2462,67 +2461,67 @@
       <c r="B1" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="32" t="s">
         <v>129</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="23" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="21" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="21" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="32" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="21" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="22" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="6" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="32" t="s">
         <v>132</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -2530,19 +2529,19 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="3" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="6" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="32" t="s">
         <v>133</v>
       </c>
       <c r="B11" s="18" t="s">
@@ -2550,25 +2549,25 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="15" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="15" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="16" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="32" t="s">
         <v>130</v>
       </c>
       <c r="B15" s="18" t="s">
@@ -2576,19 +2575,19 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="15" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="16" t="s">
         <v>150</v>
       </c>
@@ -2621,183 +2620,183 @@
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="26" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="27" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="27" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="27" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="27" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="27" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="27" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="27" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="27" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="27" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="27" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="27" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="27" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="27" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="27" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="27" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="27" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="27" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="27" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="27" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="27" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="27" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="27" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="27" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="27" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="27" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="27" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="27" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="27" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="27" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="27" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="28" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2814,7 +2813,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,45 +2831,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="19" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="C2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="A2" s="20"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>